<commit_message>
add final analyses and new files
</commit_message>
<xml_diff>
--- a/data/vercors-25-metadata.xlsx
+++ b/data/vercors-25-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPHE_enseignement\module terrain\module terrain 2025\EPHE-UE-terrain-2025\data\saison-printemps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeany\OneDrive\Documents\1-enseignements\ue-terrain\ephe-field-teaching\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8147EEB1-DF72-4F42-A700-B8ACE2C09B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFAB1A6-BC87-412E-842B-23A1022FB056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="2385" windowWidth="24135" windowHeight="15480" xr2:uid="{2EC1069D-9FAB-4063-B093-6FE4BF6F7206}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2EC1069D-9FAB-4063-B093-6FE4BF6F7206}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="32">
   <si>
     <t>SMA07072</t>
   </si>
@@ -120,6 +120,18 @@
   </si>
   <si>
     <t>Autrans-Les Gonnets</t>
+  </si>
+  <si>
+    <t>automne</t>
+  </si>
+  <si>
+    <t>SMAJYB05</t>
+  </si>
+  <si>
+    <t>SMJYB05</t>
+  </si>
+  <si>
+    <t>ete</t>
   </si>
 </sst>
 </file>
@@ -143,12 +155,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -163,11 +181,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60DCB9D-3D5B-4457-953A-3C144A1F74A8}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,49 +628,233 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="5">
         <v>45821</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="6">
         <v>0.4861111111111111</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="5">
+        <v>45821</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.52638888888888891</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G6" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1">
+        <v>45906</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>45906</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45906</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1">
+        <v>45906</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C11" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="1">
-        <v>45821</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.52638888888888891</v>
-      </c>
-      <c r="F6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
+      <c r="D11" s="1">
+        <v>45906</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.53888888888888886</v>
+      </c>
+      <c r="F11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1">
+        <v>45889</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="1">
+        <v>45889</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1">
+        <v>45889</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>